<commit_message>
Final commit for Milestone I
Project has 3 cubes drawn. Each has a crate texture with the two smaller ones acting as lights. The 3 cubes were loaded in using the FBX SDK.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{26E67174-3486-4F67-A962-884908ED76E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F98529B5-BAA5-41AB-A676-1FCAB1526F0E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -328,6 +328,12 @@
   </si>
   <si>
     <t>Student Name: Joseph Gill</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -922,7 +928,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1050,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1060,7 +1066,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1146,11 +1152,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1185,7 +1195,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
@@ -1490,11 +1500,15 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1904,11 +1918,15 @@
       <c r="D39" s="5">
         <v>4</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -1929,11 +1947,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2318,11 +2340,15 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>

</xml_diff>